<commit_message>
clean-up in prep for TSCA2019 and standardizations
</commit_message>
<xml_diff>
--- a/TSCA2019/TSCA2019_pre-processing_time_table.xlsx
+++ b/TSCA2019/TSCA2019_pre-processing_time_table.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\NHEERL_MEA\Carpenter_Amy\pre-process_mea_acute_for_tcpl\TSCA2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acarpe01\Documents\local_repos\pre-process_mea_acute_for_tcpl\TSCA2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFF951E-1C73-4893-A470-BC763376F24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0020B0-E6A3-4970-9479-219A2D314F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4E567397-73B2-48C9-9682-BA19464DA1D5}"/>
+    <workbookView xWindow="4335" yWindow="-15480" windowWidth="19440" windowHeight="14880" activeTab="1" xr2:uid="{4E567397-73B2-48C9-9682-BA19464DA1D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Totals" sheetId="2" r:id="rId2"/>
+    <sheet name="time_log" sheetId="3" r:id="rId2"/>
+    <sheet name="Totals" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$10</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>item</t>
   </si>
@@ -106,6 +107,18 @@
   </si>
   <si>
     <t>Other QC Analyses</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>time_spent</t>
+  </si>
+  <si>
+    <t>largest_category</t>
+  </si>
+  <si>
+    <t>run_me clean, debug, &amp; run</t>
   </si>
 </sst>
 </file>
@@ -472,15 +485,15 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="108.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.77734375" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -689,6 +702,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2135AE60-B10A-4D50-84BC-0F7689F34565}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>45057</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>4.57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337A8CE7-F4C3-4409-9264-A8B5176B7D77}">
   <dimension ref="A1:C3"/>
   <sheetViews>

</xml_diff>

<commit_message>
updates & clean-up as prepare TSCA2019, inc run_type update
</commit_message>
<xml_diff>
--- a/TSCA2019/TSCA2019_pre-processing_time_table.xlsx
+++ b/TSCA2019/TSCA2019_pre-processing_time_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acarpe01\Documents\local_repos\pre-process_mea_acute_for_tcpl\TSCA2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0020B0-E6A3-4970-9479-219A2D314F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0E859C-9317-4DF3-9241-0B884F5D54F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="-15480" windowWidth="19440" windowHeight="14880" activeTab="1" xr2:uid="{4E567397-73B2-48C9-9682-BA19464DA1D5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4E567397-73B2-48C9-9682-BA19464DA1D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>item</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>run_me clean, debug, &amp; run</t>
+  </si>
+  <si>
+    <t>sample ID investigation</t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,10 +706,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2135AE60-B10A-4D50-84BC-0F7689F34565}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,6 +737,28 @@
       </c>
       <c r="C2">
         <v>4.57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>45057</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>45061</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>1.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates May 26 2023 level 1-3
</commit_message>
<xml_diff>
--- a/TSCA2019/TSCA2019_pre-processing_time_table.xlsx
+++ b/TSCA2019/TSCA2019_pre-processing_time_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acarpe01\Documents\local_repos\pre-process_mea_acute_for_tcpl\TSCA2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0E859C-9317-4DF3-9241-0B884F5D54F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82BEEFD-CD48-4CE7-92BF-209EC0CFE26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4E567397-73B2-48C9-9682-BA19464DA1D5}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>item</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>sample ID investigation</t>
+  </si>
+  <si>
+    <t>detail</t>
+  </si>
+  <si>
+    <t>finalizing culture.date discrepancies; created function to read raw CTB data; worked on identifying all LDH/cyto files</t>
+  </si>
+  <si>
+    <t>finalized functions to read all raw CTB and LDH files and clean that data table; updated level 2 function</t>
+  </si>
+  <si>
+    <t>Updated lvl 2 function, updated traditional cytotox reading functions. Def not my most productive time</t>
   </si>
 </sst>
 </file>
@@ -706,63 +718,133 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2135AE60-B10A-4D50-84BC-0F7689F34565}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45057</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>4.57</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45057</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45061</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>1.78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>45068</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>45069</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>45070</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>45071</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9">
+        <v>4.42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>45072</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>1.17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
TSCA2019 updates June 2023
</commit_message>
<xml_diff>
--- a/TSCA2019/TSCA2019_pre-processing_time_table.xlsx
+++ b/TSCA2019/TSCA2019_pre-processing_time_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acarpe01\Documents\local_repos\pre-process_mea_acute_for_tcpl\TSCA2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82BEEFD-CD48-4CE7-92BF-209EC0CFE26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3DD7C3-06BB-4891-9A13-2997907D4771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4E567397-73B2-48C9-9682-BA19464DA1D5}"/>
+    <workbookView xWindow="4335" yWindow="-15480" windowWidth="19440" windowHeight="14880" activeTab="1" xr2:uid="{4E567397-73B2-48C9-9682-BA19464DA1D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>item</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Updated lvl 2 function, updated traditional cytotox reading functions. Def not my most productive time</t>
+  </si>
+  <si>
+    <t>Resolving discrepancies between raw and Calculations files cytotoxicity data</t>
   </si>
 </sst>
 </file>
@@ -718,10 +721,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2135AE60-B10A-4D50-84BC-0F7689F34565}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -840,6 +843,20 @@
       </c>
       <c r="D10">
         <v>1.17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>45082</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11">
+        <v>2.42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>